<commit_message>
validation excel file updated (formulas to parse)
</commit_message>
<xml_diff>
--- a/tmee/validation/validation_rules.xlsx
+++ b/tmee/validation/validation_rules.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beto\OneDrive\UNICEF\TransMonEE\data-etl\tmee\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{AA5BFD42-E259-4EC6-9D97-4231E348D67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{64183539-2027-4C0E-A875-E02C31753F36}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{AA5BFD42-E259-4EC6-9D97-4231E348D67F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{23FD9772-4D64-4451-85C6-16387B22958F}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{94D69724-E89C-40A6-AA5E-C46142B6A58D}"/>
   </bookViews>
@@ -638,9 +638,6 @@
     </r>
   </si>
   <si>
-    <t>40 ≥ 17, 42 ≥ 19, 43 ≥ 20, 45 ≥ 22, 62 ≥ 39</t>
-  </si>
-  <si>
     <t>The children with disabilities in formal residential care including detail disaggregation, must be less than the total children in formal residential care (never be bigger), at the end of the year. The error must be corrected (including any flag used at total or disaggregated level if necessary) or explanations must be provided in "metadata/note". Equal figures means that all children in formal residential care are children with disabilities. Equal figures can be correct for the disaggregation by age (all children in residential care of that age are children with disabilities). However, the data should be checked and confirmed.</t>
   </si>
   <si>
@@ -753,9 +750,6 @@
     </r>
   </si>
   <si>
-    <t>98 ≥ 68, 100 ≥ 70, 101 ≥ 71, 103 ≥ 73, 120 ≥ 90</t>
-  </si>
-  <si>
     <t>The children with disabilities who entered formal residential care including detail disaggregation, must be less than the total children who entered formal residential care (never be bigger), during the year. The error must be corrected (including any flag used at total or disaggregated level if necessary) or explanations must be provided in "metadata/note". Equal figures means that all children who entered formal residential care are children with disabilities. Equal figures can be correct for the disaggregation by age (all children who entered residential care of that age are children with disabilities). However, the data should be checked and confirmed.</t>
   </si>
   <si>
@@ -812,9 +806,6 @@
     </r>
   </si>
   <si>
-    <t>151 ≥ 121, 153 ≥ 123, 154 ≥ 124, 156 ≥ 126, 173 ≥ 143</t>
-  </si>
-  <si>
     <t>The children with disabilities who left formal residential care including detail disaggregation, must be less than the total children who left formal residential care (never be bigger), during the year. The error must be corrected (including any flag used at total or disaggregated level if necessary) or explanations must be provided in "metadata/note". Equal figures means that all children who left formal residential care are children with disabilities. Equal figures can be correct for the disaggregation by age (all children who left residential care of that age are children with disabilities). However, the data should be checked and confirmed.</t>
   </si>
   <si>
@@ -880,9 +871,6 @@
     <t>The test is run for all variables related to alternative care for which stock and flow data are collected. The test checks if the stock and flow data are equal. The test is failed if the data are equal (stock equal to entrants and/or stock equal to exits and/or entrants equal to exits).</t>
   </si>
   <si>
-    <t>17=68, 40=98, 17=191, 40=151, 68=191, 98=151, 63=174, 180=333, 204=357, 228=381, 280=180+204+228, 252=310, 405=180+204+228, 252=435, 180=463, 204=495, 228=527, 275=458, 280=405, 333=463, 357=495, 381=527, 310=458</t>
-  </si>
-  <si>
     <r>
       <t>Child Protection: Total number of children</t>
     </r>
@@ -1044,9 +1032,6 @@
   </si>
   <si>
     <t xml:space="preserve">The test is run for all variables for which a disaggregation which include the category "other" is collected. The test is failed when the category "other" of all relevant disaggregation is higher than 50% of the total. </t>
-  </si>
-  <si>
-    <t>category other &gt;50% of total, 97&gt;50% of 68, 150&gt;50% of 121, 309&gt;50% of 280, 434&gt;50% of 405, 494&gt;50% of 463, 526&gt;50% of 495, 558&gt;50% of 527, 683&gt;50% of 654, 713&gt;50% of 684, 743&gt;50% of 714, 773&gt;50% of 744, 853&gt;50% of 835, 872&gt;50% of 854</t>
   </si>
   <si>
     <t xml:space="preserve">The category “other" should include those not classified elsewhere and theoretically the reported figure should represent a small part of the total. The category “other" should not refer to the difference between the total and the sum of the other categories if the figures of the other categories are not available or partial. Please provide any information on "metadata/note" if necessary. Remind the category "other" should be specified by the country in "metadata/note". </t>
@@ -2506,6 +2491,21 @@
       </rPr>
       <t xml:space="preserve">To complete once the form is finalized </t>
     </r>
+  </si>
+  <si>
+    <t>40 ≥ 17, (42:43) ≥ (19:20), (45:62) ≥ (22:39)</t>
+  </si>
+  <si>
+    <t>98 ≥ 68, (100:101) ≥ (70:71), (103:120) ≥ (73:90)</t>
+  </si>
+  <si>
+    <t>151 ≥ 121, (153:154) ≥ (123:124), (156:173) ≥ (126:143)</t>
+  </si>
+  <si>
+    <t>17=68, 40=98, 17=121, 40=151, 68=121, 98=151, 63=174, 180=333, 204=357, 228=381, 280=180+204+228, 252=310, 405=180+204+228, 252=435, 180=463, 204=495, 228=527, 275=458, 280=405, 333=463, 357=495, 381=527</t>
+  </si>
+  <si>
+    <t>97&gt;50% of 68, 150&gt;50% of 121, 309&gt;50% of 280, 434&gt;50% of 405, 494&gt;50% of 463, 526&gt;50% of 495, 558&gt;50% of 527, 683&gt;50% of 654, 713&gt;50% of 684, 743&gt;50% of 714, 773&gt;50% of 744, 853&gt;50% of 835, 872&gt;50% of 854</t>
   </si>
 </sst>
 </file>
@@ -2982,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97507B5-E78C-4E50-B2D8-762FA62149D9}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3158,10 +3158,10 @@
         <v>26</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>27</v>
@@ -3184,10 +3184,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>28</v>
@@ -3210,10 +3210,10 @@
         <v>26</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>29</v>
@@ -3242,7 +3242,7 @@
         <v>134</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>135</v>
@@ -3268,7 +3268,7 @@
         <v>136</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>135</v>
@@ -3285,16 +3285,16 @@
         <v>25</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>135</v>
@@ -3320,7 +3320,7 @@
         <v>138</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>139</v>
@@ -3346,7 +3346,7 @@
         <v>141</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>139</v>
@@ -3424,10 +3424,10 @@
         <v>146</v>
       </c>
       <c r="G17" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="368" thickBot="1" x14ac:dyDescent="0.4">
@@ -3441,19 +3441,19 @@
         <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3467,19 +3467,19 @@
         <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3493,19 +3493,19 @@
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>158</v>
+        <v>321</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="368" thickBot="1" x14ac:dyDescent="0.4">
@@ -3519,22 +3519,22 @@
         <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>47</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="210.5" thickBot="1" x14ac:dyDescent="0.4">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="200" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -3545,16 +3545,16 @@
         <v>17</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>165</v>
+        <v>322</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>49</v>
@@ -3571,19 +3571,19 @@
         <v>7</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="336.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3597,19 +3597,19 @@
         <v>7</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="326" thickBot="1" x14ac:dyDescent="0.4">
@@ -3623,19 +3623,19 @@
         <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>54</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>172</v>
+        <v>323</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3649,19 +3649,19 @@
         <v>25</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="368" thickBot="1" x14ac:dyDescent="0.4">
@@ -3675,19 +3675,19 @@
         <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>56</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>57</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="326" thickBot="1" x14ac:dyDescent="0.4">
@@ -3701,19 +3701,19 @@
         <v>25</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>58</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>59</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3727,19 +3727,19 @@
         <v>25</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>60</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>61</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3753,19 +3753,19 @@
         <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3779,19 +3779,19 @@
         <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>63</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>64</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3805,19 +3805,19 @@
         <v>25</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>65</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3831,19 +3831,19 @@
         <v>25</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3857,19 +3857,19 @@
         <v>25</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>67</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3883,19 +3883,19 @@
         <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>68</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>69</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="389" thickBot="1" x14ac:dyDescent="0.4">
@@ -3909,19 +3909,19 @@
         <v>25</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="399.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3935,19 +3935,19 @@
         <v>25</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>72</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -3961,19 +3961,19 @@
         <v>25</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>73</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>74</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="294.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -3987,19 +3987,19 @@
         <v>25</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>75</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>76</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4013,19 +4013,19 @@
         <v>25</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>77</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="368" thickBot="1" x14ac:dyDescent="0.4">
@@ -4039,19 +4039,19 @@
         <v>25</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="368" thickBot="1" x14ac:dyDescent="0.4">
@@ -4065,19 +4065,19 @@
         <v>25</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>78</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="263" thickBot="1" x14ac:dyDescent="0.4">
@@ -4091,19 +4091,19 @@
         <v>7</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>79</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4117,19 +4117,19 @@
         <v>7</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>80</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G44" s="1" t="s">
         <v>81</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4143,22 +4143,22 @@
         <v>7</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>82</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="G45" s="1" t="s">
         <v>83</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="221" thickBot="1" x14ac:dyDescent="0.4">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="210.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -4169,16 +4169,16 @@
         <v>17</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>84</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>85</v>
@@ -4195,19 +4195,19 @@
         <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>87</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4221,19 +4221,19 @@
         <v>25</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="E48" s="1" t="s">
         <v>88</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>89</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="305" thickBot="1" x14ac:dyDescent="0.4">
@@ -4247,13 +4247,13 @@
         <v>25</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>90</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>91</v>
@@ -4273,19 +4273,19 @@
         <v>25</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E50" s="1" t="s">
         <v>92</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="305" thickBot="1" x14ac:dyDescent="0.4">
@@ -4299,16 +4299,16 @@
         <v>25</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>93</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>139</v>
@@ -4325,16 +4325,16 @@
         <v>25</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="E52" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>139</v>
@@ -4351,19 +4351,19 @@
         <v>25</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>95</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4377,19 +4377,19 @@
         <v>25</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>96</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4403,19 +4403,19 @@
         <v>25</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>98</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G55" s="1" t="s">
         <v>99</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4429,19 +4429,19 @@
         <v>25</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>100</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4455,19 +4455,19 @@
         <v>25</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>102</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="378.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4481,19 +4481,19 @@
         <v>7</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>103</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>104</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4507,19 +4507,19 @@
         <v>25</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>105</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4533,19 +4533,19 @@
         <v>7</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>106</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.4">
@@ -4559,19 +4559,19 @@
         <v>7</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>107</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>108</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="158" thickBot="1" x14ac:dyDescent="0.4">
@@ -4585,7 +4585,7 @@
         <v>25</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>109</v>
@@ -4597,7 +4597,7 @@
         <v>111</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="158" thickBot="1" x14ac:dyDescent="0.4">
@@ -4611,7 +4611,7 @@
         <v>25</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>112</v>
@@ -4623,7 +4623,7 @@
         <v>114</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="242" thickBot="1" x14ac:dyDescent="0.4">
@@ -4637,19 +4637,19 @@
         <v>25</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="210.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -4663,19 +4663,19 @@
         <v>25</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="E65" s="1" t="s">
         <v>116</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="221" thickBot="1" x14ac:dyDescent="0.4">
@@ -4689,7 +4689,7 @@
         <v>25</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>117</v>
@@ -4698,10 +4698,10 @@
         <v>118</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="200" thickBot="1" x14ac:dyDescent="0.4">
@@ -4715,16 +4715,16 @@
         <v>7</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>119</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="H67" s="1" t="s">
         <v>49</v>
@@ -4747,13 +4747,13 @@
         <v>122</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>123</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -4769,15 +4769,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C6C00DC80E9FED4596C9F6D7CDDD6042" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5eeea28be7a11a4fc7601b4d531de3e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="48b2e3f7-b09f-47ae-8574-fd5d5ffa6be8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="801409e539578746097a67e8a71a3340" ns2:_="">
     <xsd:import namespace="48b2e3f7-b09f-47ae-8574-fd5d5ffa6be8"/>
@@ -4949,6 +4940,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2F47DB44-C32C-4103-9CBE-22C0BABC3FC8}">
   <ds:schemaRefs>
@@ -4966,14 +4966,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{306BB486-D9C7-4C42-8994-FF856AC7670C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7AD4EBFD-F216-4EB0-8C7B-659015741667}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4989,4 +4981,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{306BB486-D9C7-4C42-8994-FF856AC7670C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>